<commit_message>
WIP 0.9.9 - Added Openplayer.js and play buttons 	modified:   BiasBuster-whisper.cmd 	modified:   KJZZ-db.py 	modified:   README.md 	modified:   kjzz/KJZZ-schedule.xlsx
</commit_message>
<xml_diff>
--- a/kjzz/KJZZ-schedule.xlsx
+++ b/kjzz/KJZZ-schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GPT\BiasBuster\kjzz\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE1E02C-F237-4B52-A94B-A324CCBFD065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCC22D2-1AF6-453B-917B-85DDD2B926B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3096" yWindow="1920" windowWidth="22164" windowHeight="12660" xr2:uid="{45C64CE4-9B74-4AA4-A561-8DD84B1E3758}"/>
+    <workbookView xWindow="3108" yWindow="1956" windowWidth="22176" windowHeight="12660" xr2:uid="{45C64CE4-9B74-4AA4-A561-8DD84B1E3758}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A21301-5EE2-4F48-BCD2-A8EB7D6452AB}">
   <dimension ref="A1:H1382"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>